<commit_message>
rename it finished report_Intro2Statistics.R
Signed-off-by: Yong-iL Joh <jsjjsmith888@gmail.com>
</commit_message>
<xml_diff>
--- a/R/DataAnalysis_with_XL.xlsx
+++ b/R/DataAnalysis_with_XL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tolkien/work/misc/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CF19F9-C62D-6C44-8DE7-DC9F23F011D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95692DA8-5868-0247-B0CA-C7F384F519BE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="460" windowWidth="26360" windowHeight="14900" activeTab="9" xr2:uid="{67B1CA6F-5820-064F-AD42-D7A4C2160BED}"/>
+    <workbookView xWindow="960" yWindow="460" windowWidth="26360" windowHeight="14900" activeTab="10" xr2:uid="{67B1CA6F-5820-064F-AD42-D7A4C2160BED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,8 @@
     <sheet name="범주형 데이터 분석" sheetId="8" r:id="rId8"/>
     <sheet name="모평균 비교" sheetId="9" r:id="rId9"/>
     <sheet name="모평균 비교.2" sheetId="11" r:id="rId10"/>
-    <sheet name="분산분석" sheetId="10" r:id="rId11"/>
+    <sheet name="모평균 비교 t-paired" sheetId="12" r:id="rId11"/>
+    <sheet name="분산분석" sheetId="10" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">고급필터!$A$5:$H$20</definedName>
@@ -69,7 +70,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId12"/>
+    <pivotCache cacheId="0" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -86,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="477">
   <si>
     <t>번호</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -3836,7 +3837,55 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{997CCEA4-703E-F24D-B476-F7A11AFE5C39}" name="피벗 테이블8" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F7BDFCAB-D9A5-9C44-A551-E814858011D8}" name="피벗 테이블2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="G5:H8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="합계 : Gender" fld="1" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{997CCEA4-703E-F24D-B476-F7A11AFE5C39}" name="피벗 테이블8" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G15:M20" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0"/>
@@ -3916,8 +3965,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{373BBE9B-40A9-9046-AC24-88C4564A3DC0}" name="피벗 테이블3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{373BBE9B-40A9-9046-AC24-88C4564A3DC0}" name="피벗 테이블3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G10:H13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0"/>
@@ -3951,54 +4000,6 @@
   </colItems>
   <dataFields count="1">
     <dataField name="합계 : Gender" fld="1" showDataAs="percentOfTotal" baseField="0" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F7BDFCAB-D9A5-9C44-A551-E814858011D8}" name="피벗 테이블2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="값" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="G5:H8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="합계 : Gender" fld="1" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -4983,10 +4984,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C83E327F-C231-D549-A63F-13BCEE8A135C}">
-  <dimension ref="A2:G43"/>
+  <dimension ref="A2:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -5183,33 +5184,33 @@
         <v>470</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="3:7">
       <c r="D17" t="s">
         <v>50</v>
       </c>
       <c r="E17">
-        <f>E6</f>
+        <f t="shared" ref="E17:F19" si="0">E6</f>
         <v>175.1</v>
       </c>
       <c r="F17">
-        <f>F6</f>
+        <f t="shared" si="0"/>
         <v>173.7</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="3:7">
       <c r="D18" t="s">
         <v>313</v>
       </c>
       <c r="E18">
-        <f>E7</f>
+        <f t="shared" si="0"/>
         <v>1831.4333333333359</v>
       </c>
       <c r="F18">
-        <f>F7</f>
+        <f t="shared" si="0"/>
         <v>184.90000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="3:7">
       <c r="C19" t="s">
         <v>329</v>
       </c>
@@ -5217,15 +5218,15 @@
         <v>314</v>
       </c>
       <c r="E19">
-        <f>E8</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F19">
-        <f>F8</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="3:7">
       <c r="D20" t="s">
         <v>323</v>
       </c>
@@ -5237,7 +5238,7 @@
         <v>40656.001111111225</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="3:7">
       <c r="C21" t="s">
         <v>330</v>
       </c>
@@ -5253,7 +5254,7 @@
         <v>3764.8178493827272</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="3:7">
       <c r="C22" t="s">
         <v>272</v>
       </c>
@@ -5265,7 +5266,7 @@
         <v>9.8593179164089884E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="3:7">
       <c r="D23" t="s">
         <v>325</v>
       </c>
@@ -5274,7 +5275,7 @@
         <v>0.46161750063056384</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="3:7">
       <c r="D24" t="s">
         <v>326</v>
       </c>
@@ -5283,7 +5284,7 @@
         <v>1.795884818704043</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="3:7">
       <c r="C25" t="s">
         <v>331</v>
       </c>
@@ -5298,7 +5299,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="19" thickBot="1">
+    <row r="26" spans="3:7" ht="19" thickBot="1">
       <c r="D26" s="22" t="s">
         <v>328</v>
       </c>
@@ -5310,212 +5311,6 @@
       <c r="G26" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" t="s">
-        <v>350</v>
-      </c>
-      <c r="C29" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" t="s">
-        <v>351</v>
-      </c>
-      <c r="B30" t="s">
-        <v>347</v>
-      </c>
-      <c r="C30" t="s">
-        <v>349</v>
-      </c>
-      <c r="D30" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="19" thickBot="1">
-      <c r="B31" s="17">
-        <v>24.7</v>
-      </c>
-      <c r="C31" s="17">
-        <v>12.4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="B32" s="17">
-        <v>46.1</v>
-      </c>
-      <c r="C32" s="17">
-        <v>14.1</v>
-      </c>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21" t="s">
-        <v>346</v>
-      </c>
-      <c r="F32" s="21" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7">
-      <c r="B33" s="17">
-        <v>18.5</v>
-      </c>
-      <c r="C33" s="17">
-        <v>7.6</v>
-      </c>
-      <c r="D33" t="s">
-        <v>50</v>
-      </c>
-      <c r="E33">
-        <v>25.736363636363635</v>
-      </c>
-      <c r="F33">
-        <v>11.899999999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7">
-      <c r="B34" s="17">
-        <v>29.5</v>
-      </c>
-      <c r="C34" s="17">
-        <v>9.5</v>
-      </c>
-      <c r="D34" t="s">
-        <v>313</v>
-      </c>
-      <c r="E34">
-        <v>69.03254545454547</v>
-      </c>
-      <c r="F34">
-        <v>12.460000000000104</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7">
-      <c r="B35" s="17">
-        <v>26.3</v>
-      </c>
-      <c r="C35" s="17">
-        <v>19.7</v>
-      </c>
-      <c r="D35" t="s">
-        <v>314</v>
-      </c>
-      <c r="E35">
-        <v>11</v>
-      </c>
-      <c r="F35">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7">
-      <c r="B36" s="17">
-        <v>33.9</v>
-      </c>
-      <c r="C36" s="17">
-        <v>10.6</v>
-      </c>
-      <c r="D36" t="s">
-        <v>353</v>
-      </c>
-      <c r="E36">
-        <v>0.25371453001499245</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7">
-      <c r="B37" s="17">
-        <v>23.1</v>
-      </c>
-      <c r="C37" s="17">
-        <v>9.1</v>
-      </c>
-      <c r="D37" t="s">
-        <v>323</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7">
-      <c r="B38" s="17">
-        <v>20.7</v>
-      </c>
-      <c r="C38" s="17">
-        <v>11.3</v>
-      </c>
-      <c r="D38" t="s">
-        <v>315</v>
-      </c>
-      <c r="E38">
-        <v>10</v>
-      </c>
-      <c r="G38" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7">
-      <c r="B39" s="17">
-        <v>18</v>
-      </c>
-      <c r="C39" s="17">
-        <v>13.3</v>
-      </c>
-      <c r="D39" t="s">
-        <v>324</v>
-      </c>
-      <c r="E39">
-        <v>5.622724632312992</v>
-      </c>
-      <c r="G39" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7">
-      <c r="B40" s="17">
-        <v>19.3</v>
-      </c>
-      <c r="C40" s="17">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="D40" t="s">
-        <v>325</v>
-      </c>
-      <c r="E40">
-        <v>1.1031198475000419E-4</v>
-      </c>
-      <c r="G40" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7">
-      <c r="B41" s="17">
-        <v>23</v>
-      </c>
-      <c r="C41" s="17">
-        <v>15</v>
-      </c>
-      <c r="D41" t="s">
-        <v>326</v>
-      </c>
-      <c r="E41">
-        <v>1.812461122811676</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7">
-      <c r="D42" t="s">
-        <v>327</v>
-      </c>
-      <c r="E42">
-        <v>2.2062396950000838E-4</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" ht="19" thickBot="1">
-      <c r="D43" s="22" t="s">
-        <v>328</v>
-      </c>
-      <c r="E43" s="22">
-        <v>2.2281388519862744</v>
-      </c>
-      <c r="F43" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -5524,6 +5319,293 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A4D910-5BEB-9342-B4DC-69F4F2ED6431}">
+  <dimension ref="A2:M18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <sheetData>
+    <row r="2" spans="1:13">
+      <c r="G2" t="s">
+        <v>350</v>
+      </c>
+      <c r="I2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B3" t="s">
+        <v>336</v>
+      </c>
+      <c r="G3" t="s">
+        <v>351</v>
+      </c>
+      <c r="H3" t="s">
+        <v>347</v>
+      </c>
+      <c r="I3" t="s">
+        <v>349</v>
+      </c>
+      <c r="J3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="19" thickBot="1">
+      <c r="B4" t="s">
+        <v>340</v>
+      </c>
+      <c r="H4" s="17">
+        <v>24.7</v>
+      </c>
+      <c r="I4" s="17">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="B5" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="H5" s="17">
+        <v>46.1</v>
+      </c>
+      <c r="I5" s="17">
+        <v>14.1</v>
+      </c>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="B6" t="s">
+        <v>338</v>
+      </c>
+      <c r="D6" t="s">
+        <v>344</v>
+      </c>
+      <c r="H6" s="17">
+        <v>18.5</v>
+      </c>
+      <c r="I6" s="17">
+        <v>7.6</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="5">
+        <v>25.736363636363635</v>
+      </c>
+      <c r="L6" s="5">
+        <v>11.899999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="B7" t="s">
+        <v>339</v>
+      </c>
+      <c r="H7" s="17">
+        <v>29.5</v>
+      </c>
+      <c r="I7" s="17">
+        <v>9.5</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="K7" s="5">
+        <v>69.03254545454547</v>
+      </c>
+      <c r="L7" s="5">
+        <v>12.460000000000104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="B8" t="s">
+        <v>272</v>
+      </c>
+      <c r="H8" s="17">
+        <v>26.3</v>
+      </c>
+      <c r="I8" s="17">
+        <v>19.7</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="K8" s="5">
+        <v>11</v>
+      </c>
+      <c r="L8" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="B9" t="s">
+        <v>341</v>
+      </c>
+      <c r="H9" s="17">
+        <v>33.9</v>
+      </c>
+      <c r="I9" s="17">
+        <v>10.6</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="K9" s="5">
+        <v>0.25371453001499245</v>
+      </c>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="B10" t="s">
+        <v>342</v>
+      </c>
+      <c r="H10" s="17">
+        <v>23.1</v>
+      </c>
+      <c r="I10" s="17">
+        <v>9.1</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="K10" s="5">
+        <v>0</v>
+      </c>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="B11" t="s">
+        <v>343</v>
+      </c>
+      <c r="H11" s="17">
+        <v>20.7</v>
+      </c>
+      <c r="I11" s="17">
+        <v>11.3</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="K11" s="5">
+        <v>10</v>
+      </c>
+      <c r="L11" s="5"/>
+      <c r="M11" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="H12" s="17">
+        <v>18</v>
+      </c>
+      <c r="I12" s="17">
+        <v>13.3</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="K12" s="5">
+        <v>5.622724632312992</v>
+      </c>
+      <c r="L12" s="5"/>
+      <c r="M12" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="C13" t="s">
+        <v>358</v>
+      </c>
+      <c r="H13" s="17">
+        <v>19.3</v>
+      </c>
+      <c r="I13" s="17">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="K13" s="5">
+        <v>1.1031198475000419E-4</v>
+      </c>
+      <c r="L13" s="5"/>
+      <c r="M13" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="C14" t="s">
+        <v>357</v>
+      </c>
+      <c r="H14" s="17">
+        <v>23</v>
+      </c>
+      <c r="I14" s="17">
+        <v>15</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="K14" s="5">
+        <v>1.812461122811676</v>
+      </c>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="C15" t="s">
+        <v>359</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="K15" s="5">
+        <v>2.2062396950000838E-4</v>
+      </c>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="1:13" ht="19" thickBot="1">
+      <c r="C16" t="s">
+        <v>356</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="K16" s="6">
+        <v>2.2281388519862744</v>
+      </c>
+      <c r="L16" s="6"/>
+    </row>
+    <row r="17" spans="3:6">
+      <c r="C17" t="s">
+        <v>360</v>
+      </c>
+      <c r="F17" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6">
+      <c r="F18" t="s">
+        <v>362</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE74125-A539-F745-BA50-841E57E9F490}">
   <dimension ref="A1:P96"/>
   <sheetViews>
@@ -9648,10 +9730,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB99346-FDFE-254D-AD15-0E551765C04C}">
-  <dimension ref="A1:O45"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -9970,7 +10052,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="3:13">
       <c r="D17" s="9" t="s">
         <v>276</v>
       </c>
@@ -9986,7 +10068,7 @@
         <v>42.25</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="3:13">
       <c r="D18" s="9" t="s">
         <v>293</v>
       </c>
@@ -10002,7 +10084,7 @@
         <v>76.38636363636364</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="3:13">
       <c r="C19" t="s">
         <v>292</v>
       </c>
@@ -10021,7 +10103,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="3:13">
       <c r="D20" s="9" t="s">
         <v>294</v>
       </c>
@@ -10037,7 +10119,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="3:13">
       <c r="J21" s="5" t="s">
         <v>323</v>
       </c>
@@ -10046,7 +10128,7 @@
       </c>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="3:13">
       <c r="J22" s="5" t="s">
         <v>315</v>
       </c>
@@ -10059,7 +10141,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="3:13">
       <c r="J23" s="5" t="s">
         <v>324</v>
       </c>
@@ -10072,7 +10154,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="3:13">
       <c r="J24" s="5" t="s">
         <v>325</v>
       </c>
@@ -10082,7 +10164,7 @@
       </c>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="3:13">
       <c r="J25" s="5" t="s">
         <v>326</v>
       </c>
@@ -10092,7 +10174,7 @@
       </c>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="3:13">
       <c r="E26" t="s">
         <v>332</v>
       </c>
@@ -10108,7 +10190,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="19" thickBot="1">
+    <row r="27" spans="3:13" ht="19" thickBot="1">
       <c r="E27" t="s">
         <v>333</v>
       </c>
@@ -10120,277 +10202,6 @@
         <v>2.0686576104190491</v>
       </c>
       <c r="L27" s="6"/>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="G29" t="s">
-        <v>350</v>
-      </c>
-      <c r="I29" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" t="s">
-        <v>335</v>
-      </c>
-      <c r="B30" t="s">
-        <v>336</v>
-      </c>
-      <c r="G30" t="s">
-        <v>351</v>
-      </c>
-      <c r="H30" t="s">
-        <v>347</v>
-      </c>
-      <c r="I30" t="s">
-        <v>349</v>
-      </c>
-      <c r="J30" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="19" thickBot="1">
-      <c r="B31" t="s">
-        <v>340</v>
-      </c>
-      <c r="H31" s="17">
-        <v>24.7</v>
-      </c>
-      <c r="I31" s="17">
-        <v>12.4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="B32" s="11" t="s">
-        <v>337</v>
-      </c>
-      <c r="H32" s="17">
-        <v>46.1</v>
-      </c>
-      <c r="I32" s="17">
-        <v>14.1</v>
-      </c>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="L32" s="7" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="33" spans="2:13">
-      <c r="B33" t="s">
-        <v>338</v>
-      </c>
-      <c r="D33" t="s">
-        <v>344</v>
-      </c>
-      <c r="H33" s="17">
-        <v>18.5</v>
-      </c>
-      <c r="I33" s="17">
-        <v>7.6</v>
-      </c>
-      <c r="J33" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="K33" s="5">
-        <v>25.736363636363635</v>
-      </c>
-      <c r="L33" s="5">
-        <v>11.899999999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="2:13">
-      <c r="B34" t="s">
-        <v>339</v>
-      </c>
-      <c r="H34" s="17">
-        <v>29.5</v>
-      </c>
-      <c r="I34" s="17">
-        <v>9.5</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="K34" s="5">
-        <v>69.03254545454547</v>
-      </c>
-      <c r="L34" s="5">
-        <v>12.460000000000104</v>
-      </c>
-    </row>
-    <row r="35" spans="2:13">
-      <c r="B35" t="s">
-        <v>272</v>
-      </c>
-      <c r="H35" s="17">
-        <v>26.3</v>
-      </c>
-      <c r="I35" s="17">
-        <v>19.7</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="K35" s="5">
-        <v>11</v>
-      </c>
-      <c r="L35" s="5">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="2:13">
-      <c r="B36" t="s">
-        <v>341</v>
-      </c>
-      <c r="H36" s="17">
-        <v>33.9</v>
-      </c>
-      <c r="I36" s="17">
-        <v>10.6</v>
-      </c>
-      <c r="J36" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="K36" s="5">
-        <v>0.25371453001499245</v>
-      </c>
-      <c r="L36" s="5"/>
-    </row>
-    <row r="37" spans="2:13">
-      <c r="B37" t="s">
-        <v>342</v>
-      </c>
-      <c r="H37" s="17">
-        <v>23.1</v>
-      </c>
-      <c r="I37" s="17">
-        <v>9.1</v>
-      </c>
-      <c r="J37" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="K37" s="5">
-        <v>0</v>
-      </c>
-      <c r="L37" s="5"/>
-    </row>
-    <row r="38" spans="2:13">
-      <c r="B38" t="s">
-        <v>343</v>
-      </c>
-      <c r="H38" s="17">
-        <v>20.7</v>
-      </c>
-      <c r="I38" s="17">
-        <v>11.3</v>
-      </c>
-      <c r="J38" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="K38" s="5">
-        <v>10</v>
-      </c>
-      <c r="L38" s="5"/>
-      <c r="M38" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="39" spans="2:13">
-      <c r="H39" s="17">
-        <v>18</v>
-      </c>
-      <c r="I39" s="17">
-        <v>13.3</v>
-      </c>
-      <c r="J39" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="K39" s="5">
-        <v>5.622724632312992</v>
-      </c>
-      <c r="L39" s="5"/>
-      <c r="M39" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="40" spans="2:13">
-      <c r="C40" t="s">
-        <v>358</v>
-      </c>
-      <c r="H40" s="17">
-        <v>19.3</v>
-      </c>
-      <c r="I40" s="17">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="J40" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="K40" s="5">
-        <v>1.1031198475000419E-4</v>
-      </c>
-      <c r="L40" s="5"/>
-      <c r="M40" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="41" spans="2:13">
-      <c r="C41" t="s">
-        <v>357</v>
-      </c>
-      <c r="H41" s="17">
-        <v>23</v>
-      </c>
-      <c r="I41" s="17">
-        <v>15</v>
-      </c>
-      <c r="J41" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="K41" s="5">
-        <v>1.812461122811676</v>
-      </c>
-      <c r="L41" s="5"/>
-    </row>
-    <row r="42" spans="2:13">
-      <c r="C42" t="s">
-        <v>359</v>
-      </c>
-      <c r="J42" s="5" t="s">
-        <v>327</v>
-      </c>
-      <c r="K42" s="5">
-        <v>2.2062396950000838E-4</v>
-      </c>
-      <c r="L42" s="5"/>
-    </row>
-    <row r="43" spans="2:13" ht="19" thickBot="1">
-      <c r="C43" t="s">
-        <v>356</v>
-      </c>
-      <c r="J43" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="K43" s="6">
-        <v>2.2281388519862744</v>
-      </c>
-      <c r="L43" s="6"/>
-    </row>
-    <row r="44" spans="2:13">
-      <c r="C44" t="s">
-        <v>360</v>
-      </c>
-      <c r="F44" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="45" spans="2:13">
-      <c r="F45" t="s">
-        <v>362</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>